<commit_message>
update to least density and dijkstra
they both now find the least cost path with densities lower than 1.0
</commit_message>
<xml_diff>
--- a/graphs.xlsx
+++ b/graphs.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,30 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjmd1g17\Documents\Fair-Vehicle-Routing-Simple-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:140008_{FF7978AF-B631-4F68-9BE9-904A250BBC92}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EC2E6146-1C89-49C9-B943-9E94B51814C5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7650" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="graphs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
   <si>
     <t>Dijkstra</t>
-  </si>
-  <si>
-    <t>RoutingType</t>
-  </si>
-  <si>
-    <t>total trips</t>
-  </si>
-  <si>
-    <t>standard dev</t>
   </si>
   <si>
     <t>avg total density</t>
@@ -45,11 +36,23 @@
   <si>
     <t>Future Dijkstra</t>
   </si>
+  <si>
+    <t>Future Least Density</t>
+  </si>
+  <si>
+    <t>vehicles sent out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard dev </t>
+  </si>
+  <si>
+    <t>avg trips completed per vehicle</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -622,11 +625,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Total</a:t>
+              <a:t>Average Number</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> trips made vs number of vehicles</a:t>
+              <a:t> of Trips Completed per Vehicle vs Number of Vehicles</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -647,8 +650,99 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Dijkstra</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>graphs!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>graphs!$B$3:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.41</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.79</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1280000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7575000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5556000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3096666666666601</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.04057142857142</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.81774999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.70755555555555505</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.59940000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-409F-4944-B006-B8281CA7C895}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="1"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>Least Density</c:v>
           </c:tx>
@@ -678,7 +772,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>graphs!$A$13:$A$22</c:f>
+              <c:f>graphs!$G$3:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -717,39 +811,39 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>graphs!$C$13:$C$22</c:f>
+              <c:f>graphs!$H$3:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1157</c:v>
+                  <c:v>2.3140000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2664</c:v>
+                  <c:v>2.6640000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3714</c:v>
+                  <c:v>2.476</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4004</c:v>
+                  <c:v>2.0019999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4171</c:v>
+                  <c:v>1.6684000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4290</c:v>
+                  <c:v>1.43</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3950</c:v>
+                  <c:v>1.1000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3664</c:v>
+                  <c:v>0.80349999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3575</c:v>
+                  <c:v>0.69444444444444398</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3211</c:v>
+                  <c:v>0.59099999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -762,14 +856,22 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
-            <c:v>Dijkstra</c:v>
+            <c:strRef>
+              <c:f>graphs!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Future Dijkstra</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>graphs!$A$2:$A$11</c:f>
+              <c:f>graphs!$M$3:$M$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -808,138 +910,39 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>graphs!$C$2:$C$11</c:f>
+              <c:f>graphs!$N$3:$N$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1205</c:v>
+                  <c:v>2.41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2790</c:v>
+                  <c:v>2.79</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3192</c:v>
+                  <c:v>2.1320000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3515</c:v>
+                  <c:v>1.847</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3889</c:v>
+                  <c:v>1.5784</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3929</c:v>
+                  <c:v>1.3656666666666599</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3645</c:v>
+                  <c:v>1.0897142857142801</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3281</c:v>
+                  <c:v>0.77900000000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3184</c:v>
+                  <c:v>0.677111111111111</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2997</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-409F-4944-B006-B8281CA7C895}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>graphs!$B$24</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Future Dijkstra</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>graphs!$A$24:$A$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2500</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4500</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>graphs!$C$24:$C$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1205</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2790</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3198</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3701</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3946</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4097</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3799</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3115</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3068</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2971</c:v>
+                  <c:v>0.59379999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -948,6 +951,105 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000C-409F-4944-B006-B8281CA7C895}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>graphs!$S$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Future Least Density</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>graphs!$S$3:$S$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>graphs!$T$3:$T$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.294</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4746666666666601</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9915</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6616</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.39333333333333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0871428571428501</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.66755555555555501</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.57120000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FF05-4B7F-9382-AB0B5F550396}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1102,11 +1204,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Number of</a:t>
+                  <a:t>Average Number of</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> trips completed </a:t>
+                  <a:t> trips completed per vehicle </a:t>
                 </a:r>
               </a:p>
               <a:p>
@@ -1241,12 +1343,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>Total</a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> trips made vs number of vehicles</a:t>
+              <a:t>Average Density vs Number of Vehicles</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1318,7 +1416,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>graphs!$A$2:$A$11</c:f>
+              <c:f>graphs!$A$3:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1357,7 +1455,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>graphs!$E$2:$E$11</c:f>
+              <c:f>graphs!$D$3:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1380,10 +1478,10 @@
                   <c:v>0.55577152777777705</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.615340277777777</c:v>
+                  <c:v>0.61559097222222203</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.64837534722222201</c:v>
+                  <c:v>0.64795538194444402</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.659918750000001</c:v>
@@ -1433,7 +1531,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>graphs!$A$13:$A$22</c:f>
+              <c:f>graphs!$G$3:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1472,7 +1570,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>graphs!$E$13:$E$22</c:f>
+              <c:f>graphs!$J$3:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1489,22 +1587,22 @@
                   <c:v>0.33372395833333302</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.39918958333333299</c:v>
+                  <c:v>0.399185590277778</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.51469947916666603</c:v>
+                  <c:v>0.51520312499999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.56781562500000005</c:v>
+                  <c:v>0.59798194444444397</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.59499531249999904</c:v>
+                  <c:v>0.63882795138888904</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.60353871527777703</c:v>
+                  <c:v>0.65642777777777805</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.61261197916666599</c:v>
+                  <c:v>0.67383645833333305</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1521,7 +1619,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>graphs!$B$24</c:f>
+              <c:f>graphs!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1556,7 +1654,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>graphs!$A$24:$A$33</c:f>
+              <c:f>graphs!$M$3:$M$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1595,7 +1693,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>graphs!$E$24:$E$33</c:f>
+              <c:f>graphs!$P$3:$P$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1606,28 +1704,28 @@
                   <c:v>0.121343749999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.24446579861111101</c:v>
+                  <c:v>0.244542361111111</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.38479201388888901</c:v>
+                  <c:v>0.383536458333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.43984305555555597</c:v>
+                  <c:v>0.43995798611111098</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.53620416666666604</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.59884965277777702</c:v>
+                  <c:v>0.60099878472222201</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.63166770833333297</c:v>
+                  <c:v>0.63591527777777801</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.64848281249999995</c:v>
+                  <c:v>0.65396197916666698</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.66124375000000102</c:v>
+                  <c:v>0.66733715277777805</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1636,6 +1734,129 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-79D2-41CE-A4D6-61A942B7DC66}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>graphs!$S$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Future Least Density</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>graphs!$S$3:$S$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>graphs!$V$3:$V$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>6.1704861111111099E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14096267361111101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.20184184027777699</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.33040364583333298</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.40023506944444398</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.51787100694444399</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.60081336805555596</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.63782638888888898</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.65715972222222196</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.66857222222222201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E019-4016-BEE3-6328D64A158A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1974,7 +2195,924 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t>Total Vehicles added to Roads vs Number of Vehicles</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Dijkstra</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>graphs!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>graphs!$E$3:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1412</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4299</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5228</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5723</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6587</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6298</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5749</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5649</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5424</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FE84-411F-A3B7-DE48252ADF40}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Least Density</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>graphs!$G$3:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>graphs!$K$3:$K$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1412</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4559</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5723</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6767</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6518</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5709</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5608</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5469</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FE84-411F-A3B7-DE48252ADF40}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>graphs!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Future Dijkstra</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>graphs!$M$3:$M$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>graphs!$Q$3:$Q$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1412</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5210</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5723</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6744</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6373</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5646</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5578</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5434</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FE84-411F-A3B7-DE48252ADF40}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>graphs!$S$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Future Least Density</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>graphs!$S$3:$S$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>graphs!$W$3:$W$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1412</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4566</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5723</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6767</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6387</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5556</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5491</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5319</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FE84-411F-A3B7-DE48252ADF40}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="334800400"/>
+        <c:axId val="333076544"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="334800400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of Vehicles</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="333076544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="333076544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Total number of vehicles added</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> to a road</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="334800400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2530,20 +3668,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>176211</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>276226</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28141</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>14721</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>51954</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2570,16 +4224,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>85727</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>90488</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1036494</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>61913</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2601,6 +4255,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>350692</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>71438</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{156A184B-1C76-46B9-9A63-1BBB19D15321}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2905,544 +4597,721 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="5" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="3" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="36.5703125" customWidth="1"/>
+    <col min="9" max="13" width="18.28515625" customWidth="1"/>
+    <col min="14" max="14" width="36.5703125" customWidth="1"/>
+    <col min="15" max="17" width="18.28515625" customWidth="1"/>
+    <col min="20" max="20" width="36.5703125" customWidth="1"/>
+    <col min="21" max="22" width="18.28515625" customWidth="1"/>
+    <col min="23" max="23" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>6</v>
+      </c>
+      <c r="S2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" t="s">
+        <v>8</v>
+      </c>
+      <c r="U2" t="s">
+        <v>7</v>
+      </c>
+      <c r="V2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>500</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3">
+        <v>2.41</v>
+      </c>
+      <c r="C3">
+        <v>0.72460340890752095</v>
+      </c>
+      <c r="D3">
+        <v>5.44838541666667E-2</v>
+      </c>
+      <c r="E3">
+        <v>1412</v>
+      </c>
+      <c r="G3">
+        <v>500</v>
+      </c>
+      <c r="H3">
+        <v>2.3140000000000001</v>
+      </c>
+      <c r="I3">
+        <v>0.79578045531800501</v>
+      </c>
+      <c r="J3">
+        <v>6.1816319444444399E-2</v>
+      </c>
+      <c r="K3">
+        <v>1412</v>
+      </c>
+      <c r="M3">
+        <v>500</v>
+      </c>
+      <c r="N3">
+        <v>2.41</v>
+      </c>
+      <c r="O3">
+        <v>0.72460340890752095</v>
+      </c>
+      <c r="P3">
+        <v>5.4453645833333397E-2</v>
+      </c>
+      <c r="Q3">
+        <v>1412</v>
+      </c>
+      <c r="S3">
+        <v>500</v>
+      </c>
+      <c r="T3">
+        <v>2.294</v>
+      </c>
+      <c r="U3">
+        <v>0.81321746494438996</v>
+      </c>
+      <c r="V3">
+        <v>6.1704861111111099E-2</v>
+      </c>
+      <c r="W3">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1000</v>
+      </c>
+      <c r="B4">
+        <v>2.79</v>
+      </c>
+      <c r="C4">
+        <v>0.50025018765638596</v>
+      </c>
+      <c r="D4">
+        <v>0.12140416666666599</v>
+      </c>
+      <c r="E4">
+        <v>3250</v>
+      </c>
+      <c r="G4">
+        <v>1000</v>
+      </c>
+      <c r="H4">
+        <v>2.6640000000000001</v>
+      </c>
+      <c r="I4">
+        <v>0.56419705628292505</v>
+      </c>
+      <c r="J4">
+        <v>0.14136874999999899</v>
+      </c>
+      <c r="K4">
+        <v>3250</v>
+      </c>
+      <c r="M4">
+        <v>1000</v>
+      </c>
+      <c r="N4">
+        <v>2.79</v>
+      </c>
+      <c r="O4">
+        <v>0.50025018765638596</v>
+      </c>
+      <c r="P4">
+        <v>0.121343749999999</v>
+      </c>
+      <c r="Q4">
+        <v>3250</v>
+      </c>
+      <c r="S4">
+        <v>1000</v>
+      </c>
+      <c r="T4">
+        <v>2.64</v>
+      </c>
+      <c r="U4">
+        <v>0.57821651164104104</v>
+      </c>
+      <c r="V4">
+        <v>0.14096267361111101</v>
+      </c>
+      <c r="W4">
+        <v>3250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1500</v>
+      </c>
+      <c r="B5">
+        <v>2.1280000000000001</v>
+      </c>
+      <c r="C5">
+        <v>0.52869620746372303</v>
+      </c>
+      <c r="D5">
+        <v>0.24308246527777699</v>
+      </c>
+      <c r="E5">
+        <v>4299</v>
+      </c>
+      <c r="G5">
+        <v>1500</v>
+      </c>
+      <c r="H5">
+        <v>2.476</v>
+      </c>
+      <c r="I5">
+        <v>0.68433340422542499</v>
+      </c>
+      <c r="J5">
+        <v>0.20223819444444399</v>
+      </c>
+      <c r="K5">
+        <v>4559</v>
+      </c>
+      <c r="M5">
+        <v>1500</v>
+      </c>
+      <c r="N5">
+        <v>2.1320000000000001</v>
+      </c>
+      <c r="O5">
+        <v>0.54485280249279799</v>
+      </c>
+      <c r="P5">
+        <v>0.244542361111111</v>
+      </c>
+      <c r="Q5">
+        <v>4365</v>
+      </c>
+      <c r="S5">
+        <v>1500</v>
+      </c>
+      <c r="T5">
+        <v>2.4746666666666601</v>
+      </c>
+      <c r="U5">
+        <v>0.69593310161342403</v>
+      </c>
+      <c r="V5">
+        <v>0.20184184027777699</v>
+      </c>
+      <c r="W5">
+        <v>4566</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2000</v>
+      </c>
+      <c r="B6">
+        <v>1.7575000000000001</v>
+      </c>
+      <c r="C6">
+        <v>5.0012504689453903E-2</v>
+      </c>
+      <c r="D6">
+        <v>0.39474930555555499</v>
+      </c>
+      <c r="E6">
+        <v>5228</v>
+      </c>
+      <c r="G6">
+        <v>2000</v>
+      </c>
+      <c r="H6">
+        <v>2.0019999999999998</v>
+      </c>
+      <c r="I6">
+        <v>0.40753287170578001</v>
+      </c>
+      <c r="J6">
+        <v>0.33372395833333302</v>
+      </c>
+      <c r="K6">
+        <v>5200</v>
+      </c>
+      <c r="M6">
+        <v>2000</v>
+      </c>
+      <c r="N6">
+        <v>1.847</v>
+      </c>
+      <c r="O6">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>1205</v>
-      </c>
-      <c r="D2">
-        <v>0.72460340890752095</v>
-      </c>
-      <c r="E2">
-        <v>5.44838541666667E-2</v>
+      <c r="P6">
+        <v>0.383536458333333</v>
+      </c>
+      <c r="Q6">
+        <v>5210</v>
+      </c>
+      <c r="S6">
+        <v>2000</v>
+      </c>
+      <c r="T6">
+        <v>1.9915</v>
+      </c>
+      <c r="U6">
+        <v>0.40383355577562502</v>
+      </c>
+      <c r="V6">
+        <v>0.33040364583333298</v>
+      </c>
+      <c r="W6">
+        <v>5200</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1000</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2500</v>
+      </c>
+      <c r="B7">
+        <v>1.5556000000000001</v>
+      </c>
+      <c r="C7">
+        <v>0.30860669992418299</v>
+      </c>
+      <c r="D7">
+        <v>0.45133767361111099</v>
+      </c>
+      <c r="E7">
+        <v>5723</v>
+      </c>
+      <c r="G7">
+        <v>2500</v>
+      </c>
+      <c r="H7">
+        <v>1.6684000000000001</v>
+      </c>
+      <c r="I7">
+        <v>0.35049841605328502</v>
+      </c>
+      <c r="J7">
+        <v>0.399185590277778</v>
+      </c>
+      <c r="K7">
+        <v>5723</v>
+      </c>
+      <c r="M7">
+        <v>2500</v>
+      </c>
+      <c r="N7">
+        <v>1.5784</v>
+      </c>
+      <c r="O7">
+        <v>0.31881131765121601</v>
+      </c>
+      <c r="P7">
+        <v>0.43995798611111098</v>
+      </c>
+      <c r="Q7">
+        <v>5723</v>
+      </c>
+      <c r="S7">
+        <v>2500</v>
+      </c>
+      <c r="T7">
+        <v>1.6616</v>
+      </c>
+      <c r="U7">
+        <v>0.35840114474178297</v>
+      </c>
+      <c r="V7">
+        <v>0.40023506944444398</v>
+      </c>
+      <c r="W7">
+        <v>5723</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3000</v>
+      </c>
+      <c r="B8">
+        <v>1.3096666666666601</v>
+      </c>
+      <c r="C8">
+        <v>0.362459826337443</v>
+      </c>
+      <c r="D8">
+        <v>0.55577152777777705</v>
+      </c>
+      <c r="E8">
+        <v>6587</v>
+      </c>
+      <c r="G8">
+        <v>3000</v>
+      </c>
+      <c r="H8">
+        <v>1.43</v>
+      </c>
+      <c r="I8">
+        <v>0.50933270717891299</v>
+      </c>
+      <c r="J8">
+        <v>0.51520312499999998</v>
+      </c>
+      <c r="K8">
+        <v>6767</v>
+      </c>
+      <c r="M8">
+        <v>3000</v>
+      </c>
+      <c r="N8">
+        <v>1.3656666666666599</v>
+      </c>
+      <c r="O8">
+        <v>0.36015261112631097</v>
+      </c>
+      <c r="P8">
+        <v>0.53620416666666604</v>
+      </c>
+      <c r="Q8">
+        <v>6744</v>
+      </c>
+      <c r="S8">
+        <v>3000</v>
+      </c>
+      <c r="T8">
+        <v>1.39333333333333</v>
+      </c>
+      <c r="U8">
+        <v>0.37733379599217698</v>
+      </c>
+      <c r="V8">
+        <v>0.51787100694444399</v>
+      </c>
+      <c r="W8">
+        <v>6767</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3500</v>
+      </c>
+      <c r="B9">
+        <v>1.04057142857142</v>
+      </c>
+      <c r="C9">
+        <v>0.38327420214851499</v>
+      </c>
+      <c r="D9">
+        <v>0.61559097222222203</v>
+      </c>
+      <c r="E9">
+        <v>6298</v>
+      </c>
+      <c r="G9">
+        <v>3500</v>
+      </c>
+      <c r="H9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I9">
+        <v>0.38327420214851499</v>
+      </c>
+      <c r="J9">
+        <v>0.59798194444444397</v>
+      </c>
+      <c r="K9">
+        <v>6518</v>
+      </c>
+      <c r="M9">
+        <v>3500</v>
+      </c>
+      <c r="N9">
+        <v>1.0897142857142801</v>
+      </c>
+      <c r="O9">
+        <v>0.38327420214851499</v>
+      </c>
+      <c r="P9">
+        <v>0.60099878472222201</v>
+      </c>
+      <c r="Q9">
+        <v>6373</v>
+      </c>
+      <c r="S9">
+        <v>3500</v>
+      </c>
+      <c r="T9">
+        <v>1.0871428571428501</v>
+      </c>
+      <c r="U9">
+        <v>0.41063317645022301</v>
+      </c>
+      <c r="V9">
+        <v>0.60081336805555596</v>
+      </c>
+      <c r="W9">
+        <v>6387</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4000</v>
+      </c>
+      <c r="B10">
+        <v>0.81774999999999998</v>
+      </c>
+      <c r="C10">
+        <v>5.2446998693137598E-2</v>
+      </c>
+      <c r="D10">
+        <v>0.64795538194444402</v>
+      </c>
+      <c r="E10">
+        <v>5749</v>
+      </c>
+      <c r="G10">
+        <v>4000</v>
+      </c>
+      <c r="H10">
+        <v>0.80349999999999999</v>
+      </c>
+      <c r="I10">
+        <v>0.23561383335792699</v>
+      </c>
+      <c r="J10">
+        <v>0.63882795138888904</v>
+      </c>
+      <c r="K10">
+        <v>5709</v>
+      </c>
+      <c r="M10">
+        <v>4000</v>
+      </c>
+      <c r="N10">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="O10">
         <v>0</v>
       </c>
-      <c r="C3">
-        <v>2790</v>
-      </c>
-      <c r="D3">
-        <v>0.50025018765638596</v>
-      </c>
-      <c r="E3">
-        <v>0.12140416666666599</v>
+      <c r="P10">
+        <v>0.63591527777777801</v>
+      </c>
+      <c r="Q10">
+        <v>5646</v>
+      </c>
+      <c r="S10">
+        <v>4000</v>
+      </c>
+      <c r="T10">
+        <v>0.76</v>
+      </c>
+      <c r="U10">
+        <v>0.165851972310189</v>
+      </c>
+      <c r="V10">
+        <v>0.63782638888888898</v>
+      </c>
+      <c r="W10">
+        <v>5556</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1500</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4500</v>
+      </c>
+      <c r="B11">
+        <v>0.70755555555555505</v>
+      </c>
+      <c r="C11">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>3192</v>
-      </c>
-      <c r="D4">
-        <v>0.52869620746372303</v>
-      </c>
-      <c r="E4">
-        <v>0.24308246527777699</v>
+      <c r="D11">
+        <v>0.659918750000001</v>
+      </c>
+      <c r="E11">
+        <v>5649</v>
+      </c>
+      <c r="G11">
+        <v>4500</v>
+      </c>
+      <c r="H11">
+        <v>0.69444444444444398</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0.65642777777777805</v>
+      </c>
+      <c r="K11">
+        <v>5608</v>
+      </c>
+      <c r="M11">
+        <v>4500</v>
+      </c>
+      <c r="N11">
+        <v>0.677111111111111</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0.65396197916666698</v>
+      </c>
+      <c r="Q11">
+        <v>5578</v>
+      </c>
+      <c r="S11">
+        <v>4500</v>
+      </c>
+      <c r="T11">
+        <v>0.66755555555555501</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0.65715972222222196</v>
+      </c>
+      <c r="W11">
+        <v>5491</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2000</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5000</v>
+      </c>
+      <c r="B12">
+        <v>0.59940000000000004</v>
+      </c>
+      <c r="C12">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>3515</v>
-      </c>
-      <c r="D5">
-        <v>5.0012504689453903E-2</v>
-      </c>
-      <c r="E5">
-        <v>0.39474930555555499</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2500</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="D12">
+        <v>0.67031250000000098</v>
+      </c>
+      <c r="E12">
+        <v>5424</v>
+      </c>
+      <c r="G12">
+        <v>5000</v>
+      </c>
+      <c r="H12">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="I12">
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>3889</v>
-      </c>
-      <c r="D6">
-        <v>0.30860669992418299</v>
-      </c>
-      <c r="E6">
-        <v>0.45133767361111099</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>3000</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="J12">
+        <v>0.67383645833333305</v>
+      </c>
+      <c r="K12">
+        <v>5469</v>
+      </c>
+      <c r="M12">
+        <v>5000</v>
+      </c>
+      <c r="N12">
+        <v>0.59379999999999999</v>
+      </c>
+      <c r="O12">
         <v>0</v>
       </c>
-      <c r="C7">
-        <v>3929</v>
-      </c>
-      <c r="D7">
-        <v>0.362459826337443</v>
-      </c>
-      <c r="E7">
-        <v>0.55577152777777705</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>3500</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="P12">
+        <v>0.66733715277777805</v>
+      </c>
+      <c r="Q12">
+        <v>5434</v>
+      </c>
+      <c r="S12">
+        <v>5000</v>
+      </c>
+      <c r="T12">
+        <v>0.57120000000000004</v>
+      </c>
+      <c r="U12">
         <v>0</v>
       </c>
-      <c r="C8">
-        <v>3645</v>
-      </c>
-      <c r="D8">
-        <v>0.38327420214851499</v>
-      </c>
-      <c r="E8">
-        <v>0.615340277777777</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>4000</v>
-      </c>
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>3281</v>
-      </c>
-      <c r="D9">
-        <v>6.7090426152472196E-2</v>
-      </c>
-      <c r="E9">
-        <v>0.64837534722222201</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>4500</v>
-      </c>
-      <c r="B10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>3184</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0.659918750000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>5000</v>
-      </c>
-      <c r="B11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>2997</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0.67031250000000098</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>500</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
-        <v>1157</v>
-      </c>
-      <c r="D13">
-        <v>0.79578045531800501</v>
-      </c>
-      <c r="E13">
-        <v>6.1816319444444399E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1000</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14">
-        <v>2664</v>
-      </c>
-      <c r="D14">
-        <v>0.56419705628292505</v>
-      </c>
-      <c r="E14">
-        <v>0.14136874999999899</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1500</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15">
-        <v>3714</v>
-      </c>
-      <c r="D15">
-        <v>0.68433340422542499</v>
-      </c>
-      <c r="E15">
-        <v>0.20223819444444399</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2000</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16">
-        <v>4004</v>
-      </c>
-      <c r="D16">
-        <v>0.40753287170578001</v>
-      </c>
-      <c r="E16">
-        <v>0.33372395833333302</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>2500</v>
-      </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17">
-        <v>4171</v>
-      </c>
-      <c r="D17">
-        <v>0.34878167879604199</v>
-      </c>
-      <c r="E17">
-        <v>0.39918958333333299</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>3000</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18">
-        <v>4290</v>
-      </c>
-      <c r="D18">
-        <v>0.50933270717891299</v>
-      </c>
-      <c r="E18">
-        <v>0.51469947916666603</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>3500</v>
-      </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19">
-        <v>3950</v>
-      </c>
-      <c r="D19">
-        <v>0.38327420214851499</v>
-      </c>
-      <c r="E19">
-        <v>0.56781562500000005</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>4000</v>
-      </c>
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20">
-        <v>3664</v>
-      </c>
-      <c r="D20">
-        <v>0.41236211104762799</v>
-      </c>
-      <c r="E20">
-        <v>0.59499531249999904</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>4500</v>
-      </c>
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21">
-        <v>3575</v>
-      </c>
-      <c r="D21">
-        <v>0.29892003880250001</v>
-      </c>
-      <c r="E21">
-        <v>0.60353871527777703</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>5000</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22">
-        <v>3211</v>
-      </c>
-      <c r="D22">
-        <v>5.4777733797812402E-2</v>
-      </c>
-      <c r="E22">
-        <v>0.61261197916666599</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>500</v>
-      </c>
-      <c r="B24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24">
-        <v>1205</v>
-      </c>
-      <c r="D24">
-        <v>0.72460340890752095</v>
-      </c>
-      <c r="E24">
-        <v>5.4453645833333397E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>1000</v>
-      </c>
-      <c r="B25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25">
-        <v>2790</v>
-      </c>
-      <c r="D25">
-        <v>0.50025018765638596</v>
-      </c>
-      <c r="E25">
-        <v>0.121343749999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>1500</v>
-      </c>
-      <c r="B26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26">
-        <v>3198</v>
-      </c>
-      <c r="D26">
-        <v>0.54485280249279799</v>
-      </c>
-      <c r="E26">
-        <v>0.24446579861111101</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>2000</v>
-      </c>
-      <c r="B27" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27">
-        <v>3701</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0.38479201388888901</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>2500</v>
-      </c>
-      <c r="B28" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28">
-        <v>3946</v>
-      </c>
-      <c r="D28">
-        <v>0.32991443953692901</v>
-      </c>
-      <c r="E28">
-        <v>0.43984305555555597</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>3000</v>
-      </c>
-      <c r="B29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29">
-        <v>4097</v>
-      </c>
-      <c r="D29">
-        <v>0.36015261112631097</v>
-      </c>
-      <c r="E29">
-        <v>0.53620416666666604</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>3500</v>
-      </c>
-      <c r="B30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30">
-        <v>3799</v>
-      </c>
-      <c r="D30">
-        <v>0.38327420214851499</v>
-      </c>
-      <c r="E30">
-        <v>0.59884965277777702</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>4000</v>
-      </c>
-      <c r="B31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31">
-        <v>3115</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>0.63166770833333297</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>4500</v>
-      </c>
-      <c r="B32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32">
-        <v>3068</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0.64848281249999995</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>5000</v>
-      </c>
-      <c r="B33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33">
-        <v>2971</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>0.66124375000000102</v>
+      <c r="V12">
+        <v>0.66857222222222201</v>
+      </c>
+      <c r="W12">
+        <v>5319</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added providing graphs through XML, tried a more complicated ex
</commit_message>
<xml_diff>
--- a/graphs.xlsx
+++ b/graphs.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjmd1g17\Documents\Fair-Vehicle-Routing-Simple-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EC2E6146-1C89-49C9-B943-9E94B51814C5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{331B975C-E9A8-4C7E-97EF-5B2535012550}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7650" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7650" tabRatio="679" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="graphs" sheetId="1" r:id="rId1"/>
+    <sheet name="graphs for street grid network" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="9">
   <si>
     <t>Dijkstra</t>
   </si>
@@ -840,7 +841,7 @@
                   <c:v>0.80349999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.69444444444444398</c:v>
+                  <c:v>0.69444444400000005</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.59099999999999997</c:v>
@@ -930,10 +931,10 @@
                   <c:v>1.5784</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3656666666666599</c:v>
+                  <c:v>1.3656666669999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0897142857142801</c:v>
+                  <c:v>1.089714286</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.77900000000000003</c:v>
@@ -1478,16 +1479,16 @@
                   <c:v>0.55577152777777705</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.61559097222222203</c:v>
+                  <c:v>0.61820937499999995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.64795538194444402</c:v>
+                  <c:v>0.65270590277777796</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.659918750000001</c:v>
+                  <c:v>0.66521354166666702</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.67031250000000098</c:v>
+                  <c:v>0.67661684027777802</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1575,34 +1576,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>6.1816319444444399E-2</c:v>
+                  <c:v>6.1816319000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14136874999999899</c:v>
+                  <c:v>0.14136874999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.20223819444444399</c:v>
+                  <c:v>0.20223819400000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.33372395833333302</c:v>
+                  <c:v>0.33372395799999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.399185590277778</c:v>
+                  <c:v>0.39918558999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.51520312499999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.59798194444444397</c:v>
+                  <c:v>0.59798194400000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.63882795138888904</c:v>
+                  <c:v>0.638827951</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.65642777777777805</c:v>
+                  <c:v>0.65642777799999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.67383645833333305</c:v>
+                  <c:v>0.67383645800000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1698,28 +1699,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>5.4453645833333397E-2</c:v>
+                  <c:v>5.4453646000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.121343749999999</c:v>
+                  <c:v>0.12134375</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.244542361111111</c:v>
+                  <c:v>0.24454236100000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.383536458333333</c:v>
+                  <c:v>0.38353645800000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.43995798611111098</c:v>
+                  <c:v>0.43995798600000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.53620416666666604</c:v>
+                  <c:v>0.53620416699999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.60099878472222201</c:v>
+                  <c:v>0.60099878500000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.63591527777777801</c:v>
+                  <c:v>0.63591527800000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.65396197916666698</c:v>
@@ -2364,16 +2365,16 @@
                   <c:v>6587</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6298</c:v>
+                  <c:v>6336</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5749</c:v>
+                  <c:v>5787</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5649</c:v>
+                  <c:v>5687</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5424</c:v>
+                  <c:v>5462</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3054,6 +3055,1946 @@
     </a:ln>
     <a:effectLst/>
   </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Standard deviation of trips</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> completed vs Number of Vehicles</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Dijkstra</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>graphs!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>graphs!$C$3:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.91409580585656802</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.81643528008444399</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.71644366679113802</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.43449757660087901</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.58501755376679598</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.69036132216440604</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.57683163968192097</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.39315846791748699</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.45493591191997101</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.490069049762063</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FCBB-457B-B007-E96111784EEB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Least Density</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>graphs!$G$3:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>graphs!$I$3:$I$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0126474759999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.889885327</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.84729133199999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.57806840599999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.61594902200000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.71035310500000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.619535269</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.518608705</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.46069352299999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.49169843800000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FCBB-457B-B007-E96111784EEB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>graphs!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Future Dijkstra</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>graphs!$M$3:$M$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>graphs!$O$3:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.91409580599999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.81643527999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.72773328299999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.36007752999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.58787045900000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.70103616599999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.61277010399999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.41497234900000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FCBB-457B-B007-E96111784EEB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>graphs!$S$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Future Least Density</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>graphs!$S$3:$S$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>graphs!$U$3:$U$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.81321746494438996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.57821651164104104</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.69593310161342403</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.40383355577562502</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.35840114474178297</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.37733379599217698</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.41063317645022301</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.165851972310189</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FCBB-457B-B007-E96111784EEB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="334800400"/>
+        <c:axId val="333076544"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="334800400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of Vehicles</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="333076544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="333076544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Standard</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> deviation of average number of trips per vehicle</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="334800400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Average Number</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> of Trips Completed per Vehicle vs Number of Vehicles</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Dijkstra</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'graphs for street grid network'!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'graphs for street grid network'!$B$3:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3.4809999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.363</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7010000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1639999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.76139999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.52233333333333298</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.40442857142857103</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35012500000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.33033333333333298</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7586-4A20-B9E2-E01DDFD8C276}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Least Density</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'graphs for street grid network'!$G$3:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'graphs for street grid network'!$H$3:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3.33</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3919999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7606666666666599</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2807500000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.89580000000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.64049999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.50857142857142801</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.44362499999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.388777777777777</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7586-4A20-B9E2-E01DDFD8C276}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'graphs for street grid network'!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Future Dijkstra</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'graphs for street grid network'!$M$3:$M$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'graphs for street grid network'!$N$3:$N$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3.5089999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4119999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.758666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2677499999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7586-4A20-B9E2-E01DDFD8C276}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'graphs for street grid network'!$S$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Future Least Density</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'graphs for street grid network'!$S$3:$S$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'graphs for street grid network'!$T$3:$T$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-7586-4A20-B9E2-E01DDFD8C276}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="334800400"/>
+        <c:axId val="333076544"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="334800400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="9000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of Vehicles</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="333076544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="333076544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Average Number of</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> trips completed per vehicle </a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t>(400 iterations)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="334800400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t>Average Road Density vs Number of Vehicles</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Dijkstra</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'graphs for street grid network'!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'graphs for street grid network'!$D$3:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.14651018772893701</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.317099324633699</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.44917995650183101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.57631196199633705</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.69209528388278296</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.78628712225274699</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.84333395146520096</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.86371919642857098</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.87364858058607997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-74FB-43A8-9987-106D8E45115F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Least Density</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'graphs for street grid network'!$G$3:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'graphs for street grid network'!$J$3:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.13677631639194099</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.299064068223443</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.427328021978022</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55273240613553098</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.66526980311355299</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.76325417811355301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.82366280906593303</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.85054532967032903</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.87113904532967001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-74FB-43A8-9987-106D8E45115F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'graphs for street grid network'!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Future Dijkstra</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'graphs for street grid network'!$M$3:$M$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'graphs for street grid network'!$P$3:$P$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.14657722100000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30482916700000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.43082781599999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.54652423299999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-74FB-43A8-9987-106D8E45115F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'graphs for street grid network'!$S$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Future Least Density</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'graphs for street grid network'!$S$3:$S$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'graphs for street grid network'!$V$3:$V$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-74FB-43A8-9987-106D8E45115F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="334800400"/>
+        <c:axId val="333076544"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="334800400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="9000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of Vehicles</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="333076544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="333076544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Average density over all roads</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="400">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>per time iteration</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="400">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-GB" baseline="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="334800400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -4298,6 +6239,125 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>280147</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>18642</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>124666</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D203E65E-26C4-4F94-A06E-16B92E877C25}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>624320</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>4763</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68157243-CDE2-415D-A82E-F9ED8E307834}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1672070</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>4763</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E8A8217-9EC6-44D3-8067-45E33FA871AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4600,8 +6660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4702,7 +6762,7 @@
         <v>2.41</v>
       </c>
       <c r="C3">
-        <v>0.72460340890752095</v>
+        <v>0.91409580585656802</v>
       </c>
       <c r="D3">
         <v>5.44838541666667E-2</v>
@@ -4717,10 +6777,10 @@
         <v>2.3140000000000001</v>
       </c>
       <c r="I3">
-        <v>0.79578045531800501</v>
+        <v>1.0126474759999999</v>
       </c>
       <c r="J3">
-        <v>6.1816319444444399E-2</v>
+        <v>6.1816319000000002E-2</v>
       </c>
       <c r="K3">
         <v>1412</v>
@@ -4732,10 +6792,10 @@
         <v>2.41</v>
       </c>
       <c r="O3">
-        <v>0.72460340890752095</v>
+        <v>0.91409580599999996</v>
       </c>
       <c r="P3">
-        <v>5.4453645833333397E-2</v>
+        <v>5.4453646000000001E-2</v>
       </c>
       <c r="Q3">
         <v>1412</v>
@@ -4764,7 +6824,7 @@
         <v>2.79</v>
       </c>
       <c r="C4">
-        <v>0.50025018765638596</v>
+        <v>0.81643528008444399</v>
       </c>
       <c r="D4">
         <v>0.12140416666666599</v>
@@ -4779,10 +6839,10 @@
         <v>2.6640000000000001</v>
       </c>
       <c r="I4">
-        <v>0.56419705628292505</v>
+        <v>0.889885327</v>
       </c>
       <c r="J4">
-        <v>0.14136874999999899</v>
+        <v>0.14136874999999999</v>
       </c>
       <c r="K4">
         <v>3250</v>
@@ -4794,10 +6854,10 @@
         <v>2.79</v>
       </c>
       <c r="O4">
-        <v>0.50025018765638596</v>
+        <v>0.81643527999999999</v>
       </c>
       <c r="P4">
-        <v>0.121343749999999</v>
+        <v>0.12134375</v>
       </c>
       <c r="Q4">
         <v>3250</v>
@@ -4826,7 +6886,7 @@
         <v>2.1280000000000001</v>
       </c>
       <c r="C5">
-        <v>0.52869620746372303</v>
+        <v>0.71644366679113802</v>
       </c>
       <c r="D5">
         <v>0.24308246527777699</v>
@@ -4841,10 +6901,10 @@
         <v>2.476</v>
       </c>
       <c r="I5">
-        <v>0.68433340422542499</v>
+        <v>0.84729133199999995</v>
       </c>
       <c r="J5">
-        <v>0.20223819444444399</v>
+        <v>0.20223819400000001</v>
       </c>
       <c r="K5">
         <v>4559</v>
@@ -4856,10 +6916,10 @@
         <v>2.1320000000000001</v>
       </c>
       <c r="O5">
-        <v>0.54485280249279799</v>
+        <v>0.72773328299999995</v>
       </c>
       <c r="P5">
-        <v>0.244542361111111</v>
+        <v>0.24454236100000001</v>
       </c>
       <c r="Q5">
         <v>4365</v>
@@ -4888,7 +6948,7 @@
         <v>1.7575000000000001</v>
       </c>
       <c r="C6">
-        <v>5.0012504689453903E-2</v>
+        <v>0.43449757660087901</v>
       </c>
       <c r="D6">
         <v>0.39474930555555499</v>
@@ -4903,10 +6963,10 @@
         <v>2.0019999999999998</v>
       </c>
       <c r="I6">
-        <v>0.40753287170578001</v>
+        <v>0.57806840599999998</v>
       </c>
       <c r="J6">
-        <v>0.33372395833333302</v>
+        <v>0.33372395799999999</v>
       </c>
       <c r="K6">
         <v>5200</v>
@@ -4918,10 +6978,10 @@
         <v>1.847</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>0.36007752999999998</v>
       </c>
       <c r="P6">
-        <v>0.383536458333333</v>
+        <v>0.38353645800000002</v>
       </c>
       <c r="Q6">
         <v>5210</v>
@@ -4950,7 +7010,7 @@
         <v>1.5556000000000001</v>
       </c>
       <c r="C7">
-        <v>0.30860669992418299</v>
+        <v>0.58501755376679598</v>
       </c>
       <c r="D7">
         <v>0.45133767361111099</v>
@@ -4965,10 +7025,10 @@
         <v>1.6684000000000001</v>
       </c>
       <c r="I7">
-        <v>0.35049841605328502</v>
+        <v>0.61594902200000001</v>
       </c>
       <c r="J7">
-        <v>0.399185590277778</v>
+        <v>0.39918558999999998</v>
       </c>
       <c r="K7">
         <v>5723</v>
@@ -4980,10 +7040,10 @@
         <v>1.5784</v>
       </c>
       <c r="O7">
-        <v>0.31881131765121601</v>
+        <v>0.58787045900000001</v>
       </c>
       <c r="P7">
-        <v>0.43995798611111098</v>
+        <v>0.43995798600000002</v>
       </c>
       <c r="Q7">
         <v>5723</v>
@@ -5012,7 +7072,7 @@
         <v>1.3096666666666601</v>
       </c>
       <c r="C8">
-        <v>0.362459826337443</v>
+        <v>0.69036132216440604</v>
       </c>
       <c r="D8">
         <v>0.55577152777777705</v>
@@ -5027,7 +7087,7 @@
         <v>1.43</v>
       </c>
       <c r="I8">
-        <v>0.50933270717891299</v>
+        <v>0.71035310500000004</v>
       </c>
       <c r="J8">
         <v>0.51520312499999998</v>
@@ -5039,13 +7099,13 @@
         <v>3000</v>
       </c>
       <c r="N8">
-        <v>1.3656666666666599</v>
+        <v>1.3656666669999999</v>
       </c>
       <c r="O8">
-        <v>0.36015261112631097</v>
+        <v>0.70103616599999996</v>
       </c>
       <c r="P8">
-        <v>0.53620416666666604</v>
+        <v>0.53620416699999995</v>
       </c>
       <c r="Q8">
         <v>6744</v>
@@ -5074,13 +7134,13 @@
         <v>1.04057142857142</v>
       </c>
       <c r="C9">
-        <v>0.38327420214851499</v>
+        <v>0.57683163968192097</v>
       </c>
       <c r="D9">
-        <v>0.61559097222222203</v>
+        <v>0.61820937499999995</v>
       </c>
       <c r="E9">
-        <v>6298</v>
+        <v>6336</v>
       </c>
       <c r="G9">
         <v>3500</v>
@@ -5089,10 +7149,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="I9">
-        <v>0.38327420214851499</v>
+        <v>0.619535269</v>
       </c>
       <c r="J9">
-        <v>0.59798194444444397</v>
+        <v>0.59798194400000004</v>
       </c>
       <c r="K9">
         <v>6518</v>
@@ -5101,13 +7161,13 @@
         <v>3500</v>
       </c>
       <c r="N9">
-        <v>1.0897142857142801</v>
+        <v>1.089714286</v>
       </c>
       <c r="O9">
-        <v>0.38327420214851499</v>
+        <v>0.61277010399999998</v>
       </c>
       <c r="P9">
-        <v>0.60099878472222201</v>
+        <v>0.60099878500000004</v>
       </c>
       <c r="Q9">
         <v>6373</v>
@@ -5136,13 +7196,13 @@
         <v>0.81774999999999998</v>
       </c>
       <c r="C10">
-        <v>5.2446998693137598E-2</v>
+        <v>0.39315846791748699</v>
       </c>
       <c r="D10">
-        <v>0.64795538194444402</v>
+        <v>0.65270590277777796</v>
       </c>
       <c r="E10">
-        <v>5749</v>
+        <v>5787</v>
       </c>
       <c r="G10">
         <v>4000</v>
@@ -5151,10 +7211,10 @@
         <v>0.80349999999999999</v>
       </c>
       <c r="I10">
-        <v>0.23561383335792699</v>
+        <v>0.518608705</v>
       </c>
       <c r="J10">
-        <v>0.63882795138888904</v>
+        <v>0.638827951</v>
       </c>
       <c r="K10">
         <v>5709</v>
@@ -5166,10 +7226,10 @@
         <v>0.77900000000000003</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>0.41497234900000002</v>
       </c>
       <c r="P10">
-        <v>0.63591527777777801</v>
+        <v>0.63591527800000003</v>
       </c>
       <c r="Q10">
         <v>5646</v>
@@ -5198,25 +7258,25 @@
         <v>0.70755555555555505</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>0.45493591191997101</v>
       </c>
       <c r="D11">
-        <v>0.659918750000001</v>
+        <v>0.66521354166666702</v>
       </c>
       <c r="E11">
-        <v>5649</v>
+        <v>5687</v>
       </c>
       <c r="G11">
         <v>4500</v>
       </c>
       <c r="H11">
-        <v>0.69444444444444398</v>
+        <v>0.69444444400000005</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>0.46069352299999999</v>
       </c>
       <c r="J11">
-        <v>0.65642777777777805</v>
+        <v>0.65642777799999996</v>
       </c>
       <c r="K11">
         <v>5608</v>
@@ -5260,13 +7320,13 @@
         <v>0.59940000000000004</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>0.490069049762063</v>
       </c>
       <c r="D12">
-        <v>0.67031250000000098</v>
+        <v>0.67661684027777802</v>
       </c>
       <c r="E12">
-        <v>5424</v>
+        <v>5462</v>
       </c>
       <c r="G12">
         <v>5000</v>
@@ -5275,10 +7335,10 @@
         <v>0.59099999999999997</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>0.49169843800000002</v>
       </c>
       <c r="J12">
-        <v>0.67383645833333305</v>
+        <v>0.67383645800000003</v>
       </c>
       <c r="K12">
         <v>5469</v>
@@ -5312,6 +7372,457 @@
       </c>
       <c r="W12">
         <v>5319</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF8D079-79BE-4296-9F31-94465D05570E}">
+  <dimension ref="A1:W11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="3" max="5" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="36.5703125" customWidth="1"/>
+    <col min="9" max="11" width="18.28515625" customWidth="1"/>
+    <col min="14" max="14" width="36.5703125" customWidth="1"/>
+    <col min="15" max="17" width="18.28515625" customWidth="1"/>
+    <col min="20" max="20" width="36.5703125" customWidth="1"/>
+    <col min="21" max="23" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>6</v>
+      </c>
+      <c r="S2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" t="s">
+        <v>8</v>
+      </c>
+      <c r="U2" t="s">
+        <v>7</v>
+      </c>
+      <c r="V2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1000</v>
+      </c>
+      <c r="B3">
+        <v>3.4809999999999999</v>
+      </c>
+      <c r="C3">
+        <v>2.9292011230400599</v>
+      </c>
+      <c r="D3">
+        <v>0.14651018772893701</v>
+      </c>
+      <c r="E3">
+        <v>4376</v>
+      </c>
+      <c r="G3">
+        <v>1000</v>
+      </c>
+      <c r="H3">
+        <v>3.33</v>
+      </c>
+      <c r="I3">
+        <v>3.0878203695543198</v>
+      </c>
+      <c r="J3">
+        <v>0.13677631639194099</v>
+      </c>
+      <c r="K3">
+        <v>4222</v>
+      </c>
+      <c r="M3">
+        <v>1000</v>
+      </c>
+      <c r="N3">
+        <v>3.5089999999999999</v>
+      </c>
+      <c r="O3">
+        <v>2.935393591</v>
+      </c>
+      <c r="P3">
+        <v>0.14657722100000001</v>
+      </c>
+      <c r="Q3">
+        <v>4403</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2000</v>
+      </c>
+      <c r="B4">
+        <v>2.363</v>
+      </c>
+      <c r="C4">
+        <v>2.3603000886019099</v>
+      </c>
+      <c r="D4">
+        <v>0.317099324633699</v>
+      </c>
+      <c r="E4">
+        <v>6512</v>
+      </c>
+      <c r="G4">
+        <v>2000</v>
+      </c>
+      <c r="H4">
+        <v>2.3919999999999999</v>
+      </c>
+      <c r="I4">
+        <v>2.4609681391864799</v>
+      </c>
+      <c r="J4">
+        <v>0.299064068223443</v>
+      </c>
+      <c r="K4">
+        <v>6566</v>
+      </c>
+      <c r="M4">
+        <v>2000</v>
+      </c>
+      <c r="N4">
+        <v>2.4119999999999999</v>
+      </c>
+      <c r="O4">
+        <v>2.4364367649999998</v>
+      </c>
+      <c r="P4">
+        <v>0.30482916700000001</v>
+      </c>
+      <c r="Q4">
+        <v>6452</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3000</v>
+      </c>
+      <c r="B5">
+        <v>1.7010000000000001</v>
+      </c>
+      <c r="C5">
+        <v>2.0566175041847998</v>
+      </c>
+      <c r="D5">
+        <v>0.44917995650183101</v>
+      </c>
+      <c r="E5">
+        <v>7777</v>
+      </c>
+      <c r="G5">
+        <v>3000</v>
+      </c>
+      <c r="H5">
+        <v>1.7606666666666599</v>
+      </c>
+      <c r="I5">
+        <v>2.2464197491680298</v>
+      </c>
+      <c r="J5">
+        <v>0.427328021978022</v>
+      </c>
+      <c r="K5">
+        <v>7916</v>
+      </c>
+      <c r="M5">
+        <v>3000</v>
+      </c>
+      <c r="N5">
+        <v>1.758666667</v>
+      </c>
+      <c r="O5">
+        <v>2.129930458</v>
+      </c>
+      <c r="P5">
+        <v>0.43082781599999997</v>
+      </c>
+      <c r="Q5">
+        <v>7667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4000</v>
+      </c>
+      <c r="B6">
+        <v>1.1639999999999999</v>
+      </c>
+      <c r="C6">
+        <v>1.77042017524071</v>
+      </c>
+      <c r="D6">
+        <v>0.57631196199633705</v>
+      </c>
+      <c r="E6">
+        <v>8238</v>
+      </c>
+      <c r="G6">
+        <v>4000</v>
+      </c>
+      <c r="H6">
+        <v>1.2807500000000001</v>
+      </c>
+      <c r="I6">
+        <v>2.0446208832296402</v>
+      </c>
+      <c r="J6">
+        <v>0.55273240613553098</v>
+      </c>
+      <c r="K6">
+        <v>8687</v>
+      </c>
+      <c r="M6">
+        <v>4000</v>
+      </c>
+      <c r="N6">
+        <v>1.2677499999999999</v>
+      </c>
+      <c r="O6">
+        <v>1.72127878</v>
+      </c>
+      <c r="P6">
+        <v>0.54652423299999997</v>
+      </c>
+      <c r="Q6">
+        <v>8346</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5000</v>
+      </c>
+      <c r="B7">
+        <v>0.76139999999999997</v>
+      </c>
+      <c r="C7">
+        <v>1.41282315023881</v>
+      </c>
+      <c r="D7">
+        <v>0.69209528388278296</v>
+      </c>
+      <c r="E7">
+        <v>8254</v>
+      </c>
+      <c r="G7">
+        <v>5000</v>
+      </c>
+      <c r="H7">
+        <v>0.89580000000000004</v>
+      </c>
+      <c r="I7">
+        <v>1.7078424122679201</v>
+      </c>
+      <c r="J7">
+        <v>0.66526980311355299</v>
+      </c>
+      <c r="K7">
+        <v>8965</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6000</v>
+      </c>
+      <c r="B8">
+        <v>0.52233333333333298</v>
+      </c>
+      <c r="C8">
+        <v>1.0511987087810699</v>
+      </c>
+      <c r="D8">
+        <v>0.78628712225274699</v>
+      </c>
+      <c r="E8">
+        <v>8303</v>
+      </c>
+      <c r="G8">
+        <v>6000</v>
+      </c>
+      <c r="H8">
+        <v>0.64049999999999996</v>
+      </c>
+      <c r="I8">
+        <v>1.3594978689731601</v>
+      </c>
+      <c r="J8">
+        <v>0.76325417811355301</v>
+      </c>
+      <c r="K8">
+        <v>9068</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7000</v>
+      </c>
+      <c r="B9">
+        <v>0.40442857142857103</v>
+      </c>
+      <c r="C9">
+        <v>0.89177655591134197</v>
+      </c>
+      <c r="D9">
+        <v>0.84333395146520096</v>
+      </c>
+      <c r="E9">
+        <v>8567</v>
+      </c>
+      <c r="G9">
+        <v>7000</v>
+      </c>
+      <c r="H9">
+        <v>0.50857142857142801</v>
+      </c>
+      <c r="I9">
+        <v>1.1546687202174</v>
+      </c>
+      <c r="J9">
+        <v>0.82366280906593303</v>
+      </c>
+      <c r="K9">
+        <v>9240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8000</v>
+      </c>
+      <c r="B10">
+        <v>0.35012500000000002</v>
+      </c>
+      <c r="C10">
+        <v>0.84343132881453897</v>
+      </c>
+      <c r="D10">
+        <v>0.86371919642857098</v>
+      </c>
+      <c r="E10">
+        <v>8844</v>
+      </c>
+      <c r="G10">
+        <v>8000</v>
+      </c>
+      <c r="H10">
+        <v>0.44362499999999999</v>
+      </c>
+      <c r="I10">
+        <v>1.04496811155617</v>
+      </c>
+      <c r="J10">
+        <v>0.85054532967032903</v>
+      </c>
+      <c r="K10">
+        <v>9519</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9000</v>
+      </c>
+      <c r="B11">
+        <v>0.33033333333333298</v>
+      </c>
+      <c r="C11">
+        <v>0.85502761958190099</v>
+      </c>
+      <c r="D11">
+        <v>0.87364858058607997</v>
+      </c>
+      <c r="E11">
+        <v>9070</v>
+      </c>
+      <c r="G11">
+        <v>9000</v>
+      </c>
+      <c r="H11">
+        <v>0.388777777777777</v>
+      </c>
+      <c r="I11">
+        <v>0.93139883206453</v>
+      </c>
+      <c r="J11">
+        <v>0.87113904532967001</v>
+      </c>
+      <c r="K11">
+        <v>9721</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changing stats tracking methods
</commit_message>
<xml_diff>
--- a/graphs.xlsx
+++ b/graphs.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjmd1g17\Documents\Fair-Vehicle-Routing-Simple-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{331B975C-E9A8-4C7E-97EF-5B2535012550}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BBDD1CE8-9FBD-4102-A1FB-FD784C4613BA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7650" tabRatio="679" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="graphs" sheetId="1" r:id="rId1"/>
     <sheet name="graphs for street grid network" sheetId="2" r:id="rId2"/>
+    <sheet name="graphs for Berlin network" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="10">
   <si>
     <t>Dijkstra</t>
   </si>
@@ -48,6 +49,9 @@
   </si>
   <si>
     <t>avg trips completed per vehicle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -4933,6 +4937,1766 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-GB" baseline="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="334800400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Average Number</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> of Trips Completed per Vehicle vs Number of Vehicles</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Dijkstra</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'graphs for Berlin network'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'graphs for Berlin network'!$B$3:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>15.87</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.2285000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.1920000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5194999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4018000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9390000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.72257142857142</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5238750000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4526666666666599</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-25C3-4E53-A447-BAC166D4A8D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Least Density</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'graphs for Berlin network'!$G$3:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'graphs for Berlin network'!$H$3:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>21.41</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.964499999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.17766666666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4690000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0872000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5651666666666602</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1872857142857098</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.841375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7528888888888801</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-25C3-4E53-A447-BAC166D4A8D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'graphs for street grid network'!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Future Dijkstra</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'graphs for Berlin network'!$M$3:$M$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'graphs for Berlin network'!$N$3:$N$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-25C3-4E53-A447-BAC166D4A8D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'graphs for street grid network'!$S$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Future Least Density</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'graphs for street grid network'!$S$3:$S$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'graphs for street grid network'!$T$3:$T$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-25C3-4E53-A447-BAC166D4A8D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="334800400"/>
+        <c:axId val="333076544"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="334800400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="9000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of Vehicles</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="333076544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="333076544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Average Number of</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> trips completed per vehicle </a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t>(400 iterations)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="334800400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t>Average Road Density vs Number of Vehicles</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Dijkstra</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'graphs for Berlin network'!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'graphs for Berlin network'!$D$3:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.17143720012626201</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.34785347748316398</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.471372767606621</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.557103072390572</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.63530660949775497</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.68215195882435398</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.71856367494388296</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.74913255997474704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.76420237443883199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0E3C-4AC9-9418-3DB98A329F98}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Least Density</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'graphs for Berlin network'!$G$3:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'graphs for Berlin network'!$J$3:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.104015570636924</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25819824810606001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.39358250911896703</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.53575385451739599</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.61273096766273805</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.66416751017115505</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.70137518237934804</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.72661918139730597</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.74047975939955102</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0E3C-4AC9-9418-3DB98A329F98}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'graphs for street grid network'!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Future Dijkstra</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'graphs for Berlin network'!$M$3:$M$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'graphs for Berlin network'!$P$3:$P$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0E3C-4AC9-9418-3DB98A329F98}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'graphs for street grid network'!$S$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Future Least Density</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'graphs for street grid network'!$S$3:$S$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'graphs for street grid network'!$V$3:$V$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0E3C-4AC9-9418-3DB98A329F98}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="334800400"/>
+        <c:axId val="333076544"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="334800400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="9000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of Vehicles</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="333076544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="333076544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Average density over all roads</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="400">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>per time iteration</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="400">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-GB" baseline="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="334800400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Standard deviation of trips</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> completed vs Number of Vehicles</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Dijkstra</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'graphs for Berlin network'!$A$3:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'graphs for Berlin network'!$C$3:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>28.6528547632882</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.384922376112598</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.9213577481374</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.7494098536044</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.0650592568331</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.4013302162495194</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.2380469118985697</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.9394585531939494</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.8317472523181202</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0579-45B7-A851-95607E3678A7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Least Density</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'graphs for Berlin network'!$G$3:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'graphs for Berlin network'!$I$3:$I$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>30.2456393336081</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.4977326774627</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.586016557526399</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.320713169715701</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.115066581043401</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.362655424471599</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.7690657586969</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.2856787577586</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.362055764977899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0579-45B7-A851-95607E3678A7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>graphs!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Future Dijkstra</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'graphs for Berlin network'!$M$3:$M$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'graphs for Berlin network'!$O$3:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0579-45B7-A851-95607E3678A7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>graphs!$S$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Future Least Density</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'graphs for Berlin network'!$S$3:$S$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'graphs for Berlin network'!$U$3:$U$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0579-45B7-A851-95607E3678A7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="334800400"/>
+        <c:axId val="333076544"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="334800400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of Vehicles</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="333076544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="333076544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Standard</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> deviation of average number of trips per vehicle</a:t>
+                </a:r>
               </a:p>
             </c:rich>
           </c:tx>
@@ -6361,6 +8125,125 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>462395</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>52388</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{290EA4A7-6D56-47AE-ADDD-83A9A660935B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1510145</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>52388</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CD5278F-489F-4037-947E-B5CB768517AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>500495</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>138113</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1E74C3A-D85B-44D4-BC0A-B3BE6964EC38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6661,7 +8544,7 @@
   <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7385,7 +9268,7 @@
   <dimension ref="A1:W11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7829,4 +9712,399 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16AA9883-A9B7-46BD-8BA2-2CDD2C033432}">
+  <dimension ref="A1:W45"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="3" max="5" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="36.5703125" customWidth="1"/>
+    <col min="9" max="11" width="18.28515625" customWidth="1"/>
+    <col min="14" max="14" width="36.5703125" customWidth="1"/>
+    <col min="15" max="17" width="18.28515625" customWidth="1"/>
+    <col min="20" max="20" width="36.5703125" customWidth="1"/>
+    <col min="21" max="23" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>6</v>
+      </c>
+      <c r="S2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" t="s">
+        <v>8</v>
+      </c>
+      <c r="U2" t="s">
+        <v>7</v>
+      </c>
+      <c r="V2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1000</v>
+      </c>
+      <c r="B3">
+        <v>15.87</v>
+      </c>
+      <c r="C3">
+        <v>28.6528547632882</v>
+      </c>
+      <c r="D3">
+        <v>0.17143720012626201</v>
+      </c>
+      <c r="E3">
+        <v>16787</v>
+      </c>
+      <c r="G3">
+        <v>1000</v>
+      </c>
+      <c r="H3">
+        <v>21.41</v>
+      </c>
+      <c r="I3">
+        <v>30.2456393336081</v>
+      </c>
+      <c r="J3">
+        <v>0.104015570636924</v>
+      </c>
+      <c r="K3">
+        <v>22321</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2000</v>
+      </c>
+      <c r="B4">
+        <v>9.2285000000000004</v>
+      </c>
+      <c r="C4">
+        <v>20.384922376112598</v>
+      </c>
+      <c r="D4">
+        <v>0.34785347748316398</v>
+      </c>
+      <c r="E4">
+        <v>20319</v>
+      </c>
+      <c r="G4">
+        <v>2000</v>
+      </c>
+      <c r="H4">
+        <v>14.964499999999999</v>
+      </c>
+      <c r="I4">
+        <v>27.4977326774627</v>
+      </c>
+      <c r="J4">
+        <v>0.25819824810606001</v>
+      </c>
+      <c r="K4">
+        <v>31752</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3000</v>
+      </c>
+      <c r="B5">
+        <v>5.1920000000000002</v>
+      </c>
+      <c r="C5">
+        <v>15.9213577481374</v>
+      </c>
+      <c r="D5">
+        <v>0.471372767606621</v>
+      </c>
+      <c r="E5">
+        <v>18362</v>
+      </c>
+      <c r="G5">
+        <v>3000</v>
+      </c>
+      <c r="H5">
+        <v>9.17766666666666</v>
+      </c>
+      <c r="I5">
+        <v>22.586016557526399</v>
+      </c>
+      <c r="J5">
+        <v>0.39358250911896703</v>
+      </c>
+      <c r="K5">
+        <v>30247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4000</v>
+      </c>
+      <c r="B6">
+        <v>3.5194999999999999</v>
+      </c>
+      <c r="C6">
+        <v>11.7494098536044</v>
+      </c>
+      <c r="D6">
+        <v>0.557103072390572</v>
+      </c>
+      <c r="E6">
+        <v>17636</v>
+      </c>
+      <c r="G6">
+        <v>4000</v>
+      </c>
+      <c r="H6">
+        <v>4.4690000000000003</v>
+      </c>
+      <c r="I6">
+        <v>13.320713169715701</v>
+      </c>
+      <c r="J6">
+        <v>0.53575385451739599</v>
+      </c>
+      <c r="K6">
+        <v>21495</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5000</v>
+      </c>
+      <c r="B7">
+        <v>2.4018000000000002</v>
+      </c>
+      <c r="C7">
+        <v>10.0650592568331</v>
+      </c>
+      <c r="D7">
+        <v>0.63530660949775497</v>
+      </c>
+      <c r="E7">
+        <v>16381</v>
+      </c>
+      <c r="G7">
+        <v>5000</v>
+      </c>
+      <c r="H7">
+        <v>3.0872000000000002</v>
+      </c>
+      <c r="I7">
+        <v>11.115066581043401</v>
+      </c>
+      <c r="J7">
+        <v>0.61273096766273805</v>
+      </c>
+      <c r="K7">
+        <v>19730</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6000</v>
+      </c>
+      <c r="B8">
+        <v>1.9390000000000001</v>
+      </c>
+      <c r="C8">
+        <v>9.4013302162495194</v>
+      </c>
+      <c r="D8">
+        <v>0.68215195882435398</v>
+      </c>
+      <c r="E8">
+        <v>16654</v>
+      </c>
+      <c r="G8">
+        <v>6000</v>
+      </c>
+      <c r="H8">
+        <v>2.5651666666666602</v>
+      </c>
+      <c r="I8">
+        <v>11.362655424471599</v>
+      </c>
+      <c r="J8">
+        <v>0.66416751017115505</v>
+      </c>
+      <c r="K8">
+        <v>20463</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7000</v>
+      </c>
+      <c r="B9">
+        <v>1.72257142857142</v>
+      </c>
+      <c r="C9">
+        <v>9.2380469118985697</v>
+      </c>
+      <c r="D9">
+        <v>0.71856367494388296</v>
+      </c>
+      <c r="E9">
+        <v>17613</v>
+      </c>
+      <c r="G9">
+        <v>7000</v>
+      </c>
+      <c r="H9">
+        <v>2.1872857142857098</v>
+      </c>
+      <c r="I9">
+        <v>10.7690657586969</v>
+      </c>
+      <c r="J9">
+        <v>0.70137518237934804</v>
+      </c>
+      <c r="K9">
+        <v>20785</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8000</v>
+      </c>
+      <c r="B10">
+        <v>1.5238750000000001</v>
+      </c>
+      <c r="C10">
+        <v>8.9394585531939494</v>
+      </c>
+      <c r="D10">
+        <v>0.74913255997474704</v>
+      </c>
+      <c r="E10">
+        <v>18192</v>
+      </c>
+      <c r="G10">
+        <v>8000</v>
+      </c>
+      <c r="H10">
+        <v>1.841375</v>
+      </c>
+      <c r="I10">
+        <v>10.2856787577586</v>
+      </c>
+      <c r="J10">
+        <v>0.72661918139730597</v>
+      </c>
+      <c r="K10">
+        <v>20573</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9000</v>
+      </c>
+      <c r="B11">
+        <v>1.4526666666666599</v>
+      </c>
+      <c r="C11">
+        <v>8.8317472523181202</v>
+      </c>
+      <c r="D11">
+        <v>0.76420237443883199</v>
+      </c>
+      <c r="E11">
+        <v>19308</v>
+      </c>
+      <c r="G11">
+        <v>9000</v>
+      </c>
+      <c r="H11">
+        <v>1.7528888888888801</v>
+      </c>
+      <c r="I11">
+        <v>10.362055764977899</v>
+      </c>
+      <c r="J11">
+        <v>0.74047975939955102</v>
+      </c>
+      <c r="K11">
+        <v>21869</v>
+      </c>
+    </row>
+    <row r="45" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>